<commit_message>
added stores for sewing
</commit_message>
<xml_diff>
--- a/Final_Project/Einzelhandel_Template.xlsx
+++ b/Final_Project/Einzelhandel_Template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="143">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -425,6 +425,30 @@
   </si>
   <si>
     <t xml:space="preserve">4.1/5 (99)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stoff-Art</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eisfeld 3, 99423 Weimar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.8/5 (46)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stoffgeschäft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verfilzt &amp; Zugenäht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jakobstraße 2, 99423 Weimar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mo – Fr 11:00 – 17:00, Sa 11:00 – 15:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.9/5 (39)</t>
   </si>
 </sst>
 </file>
@@ -532,11 +556,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -559,8 +583,8 @@
   </sheetPr>
   <dimension ref="B2:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.57421875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1021,7 +1045,7 @@
       <c r="C24" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="1" t="s">
         <v>92</v>
       </c>
       <c r="E24" s="1" t="n">
@@ -1061,7 +1085,7 @@
       <c r="C26" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="1" t="s">
         <v>104</v>
       </c>
       <c r="E26" s="1" t="s">
@@ -1101,7 +1125,7 @@
       <c r="C28" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="1" t="s">
         <v>113</v>
       </c>
       <c r="E28" s="1" t="s">
@@ -1127,7 +1151,7 @@
       <c r="E29" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F29" s="1" t="s">
         <v>118</v>
       </c>
       <c r="G29" s="1" t="s">
@@ -1164,7 +1188,7 @@
       <c r="D31" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E31" s="5" t="n">
+      <c r="E31" s="4" t="n">
         <v>0.625</v>
       </c>
       <c r="F31" s="1" t="s">
@@ -1181,7 +1205,7 @@
       <c r="C32" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="1" t="s">
         <v>129</v>
       </c>
       <c r="E32" s="1" t="n">
@@ -1212,6 +1236,46 @@
       </c>
       <c r="G33" s="1" t="s">
         <v>110</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E34" s="4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>